<commit_message>
1. Data slicing bug fixed for SimpleFedDataLoader; 2. Shuffle added to SimpleFedDataLoader, untested; 3. Some args temporarily replaced with external cmd argvs
</commit_message>
<xml_diff>
--- a/stats/exp_stats.xlsx
+++ b/stats/exp_stats.xlsx
@@ -11,6 +11,7 @@
     <sheet name="Reg" sheetId="1" r:id="rId2"/>
     <sheet name="SVM" sheetId="2" r:id="rId3"/>
     <sheet name="CNN" sheetId="3" r:id="rId4"/>
+    <sheet name="traces" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="53">
   <si>
     <t>C = 0.1</t>
   </si>
@@ -78,29 +79,176 @@
     <t>lag_t=5</t>
   </si>
   <si>
-    <t>acc / at round #</t>
-  </si>
-  <si>
-    <t>crash=0.1</t>
-  </si>
-  <si>
-    <t>SAFA, Reg (C=0.5, B= , E=)</t>
-  </si>
-  <si>
-    <t>SAFA, SVM (C=0.5, B= , E=)</t>
-  </si>
-  <si>
     <t>SAFA, CNN (C=0.5, B= , E=)</t>
+  </si>
+  <si>
+    <t>mu = N/M</t>
+  </si>
+  <si>
+    <t>Crash_prob=E</t>
+  </si>
+  <si>
+    <t>crash_prob</t>
+  </si>
+  <si>
+    <t>lr</t>
+  </si>
+  <si>
+    <t>D~N(mu, 0.3*mu)</t>
+  </si>
+  <si>
+    <t>SAFA, Reg (M=5, R= 50, E=3, B=5, C=0.5)</t>
+  </si>
+  <si>
+    <t>best loss / at round #</t>
+  </si>
+  <si>
+    <t>0.0315/44</t>
+  </si>
+  <si>
+    <t>0.819/49</t>
+  </si>
+  <si>
+    <t>0.704/49</t>
+  </si>
+  <si>
+    <t>0.0315/40</t>
+  </si>
+  <si>
+    <t>0.0316/39</t>
+  </si>
+  <si>
+    <t>0.0315/47</t>
+  </si>
+  <si>
+    <t>0.0314/64</t>
+  </si>
+  <si>
+    <t>0.0315/57</t>
+  </si>
+  <si>
+    <t>0.0316/53</t>
+  </si>
+  <si>
+    <t>0.0315/64</t>
+  </si>
+  <si>
+    <t>0.0314/55</t>
+  </si>
+  <si>
+    <t>0.0315/91</t>
+  </si>
+  <si>
+    <t>0.0315/79</t>
+  </si>
+  <si>
+    <t>0.0314/79</t>
+  </si>
+  <si>
+    <t>0.0315/75</t>
+  </si>
+  <si>
+    <t>0.0316/74</t>
+  </si>
+  <si>
+    <t>0.0408/98</t>
+  </si>
+  <si>
+    <t>0.0369/99</t>
+  </si>
+  <si>
+    <t>0.0339/99</t>
+  </si>
+  <si>
+    <t>0.0317/98</t>
+  </si>
+  <si>
+    <t>0.0375/99</t>
+  </si>
+  <si>
+    <t>0.623/49</t>
+  </si>
+  <si>
+    <t>C=0.5</t>
+  </si>
+  <si>
+    <t>0.559/49</t>
+  </si>
+  <si>
+    <t>0.564/49</t>
+  </si>
+  <si>
+    <t>0.305/99</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SAFA, SVM (M=500, R= </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, E=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, B=100, C=0.5)</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,7 +274,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -137,6 +285,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -417,189 +576,308 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="H2" s="4">
+        <v>1E-4</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>16</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+        <v>0.5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>0.7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="H10" s="4">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="2" t="s">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s">
+        <v>49</v>
+      </c>
+      <c r="F12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="H17" s="4">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F18" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>0.7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>0.7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A10:F10"/>
+    <mergeCell ref="A17:F17"/>
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N33"/>
+  <dimension ref="A2:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A15" sqref="A15:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,40 +887,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="I2" s="3" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="I3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -715,22 +993,22 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="I9" s="3" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="I9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -802,127 +1080,127 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="A22" s="1">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A28" s="1">
         <v>0.7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="I3:N3"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="A17:F17"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="I9:N9"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="I3:N3"/>
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="I2:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -931,10 +1209,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N33"/>
+  <dimension ref="A2:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,40 +1222,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="I2" s="3" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="I3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1050,22 +1328,22 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="I9" s="3" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="I9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1137,121 +1415,121 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="A22" s="1">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A28" s="1">
         <v>0.7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A23:F23"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="A3:F3"/>
@@ -1266,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:N33"/>
+  <dimension ref="A2:N28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1279,40 +1557,40 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="I2" s="3" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="I2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="I3" s="3" t="s">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="I3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1385,22 +1663,22 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="I9" s="3" t="s">
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="I9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1472,121 +1750,121 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>0.3</v>
+      </c>
+    </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="1">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="A22" s="1">
+        <v>0.7</v>
+      </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="B24" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
-        <v>0.3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A28" s="1">
         <v>0.7</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A17:F17"/>
+    <mergeCell ref="A23:F23"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="I2:N2"/>
     <mergeCell ref="A3:F3"/>
@@ -1597,4 +1875,16 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
FL framework refractored using local client and data support in place of PySyft
</commit_message>
<xml_diff>
--- a/stats/exp_stats.xlsx
+++ b/stats/exp_stats.xlsx
@@ -1820,7 +1820,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1832,10 +1839,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1845,9 +1852,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1862,10 +1866,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1923,7 +1923,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2472,7 +2471,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2586,7 +2584,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3234,7 +3231,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3983,7 +3979,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9155,7 +9150,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9703,7 +9697,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -9818,7 +9811,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10366,7 +10358,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10478,7 +10469,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -11026,7 +11016,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12171,7 +12160,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13128,7 +13116,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -14259,7 +14246,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15170,7 +15156,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -25704,14 +25689,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
       <c r="H1" t="s">
         <v>15</v>
       </c>
@@ -25726,14 +25711,14 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
       <c r="H2" s="4">
         <v>1E-4</v>
       </c>
@@ -25742,14 +25727,14 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -25869,14 +25854,14 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -25996,14 +25981,14 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="61" t="s">
+      <c r="A17" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="61"/>
+      <c r="B17" s="62"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="62"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
@@ -26118,28 +26103,28 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="57"/>
-      <c r="H25" s="57"/>
-      <c r="I25" s="57"/>
-      <c r="J25" s="57"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="61"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
       <c r="G26" s="7" t="s">
         <v>164</v>
       </c>
@@ -26154,28 +26139,28 @@
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="57" t="s">
+      <c r="A27" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="57"/>
-      <c r="C27" s="57"/>
-      <c r="D27" s="57"/>
-      <c r="E27" s="57"/>
-      <c r="F27" s="57"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
       <c r="G27" s="7"/>
       <c r="I27" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="57" t="s">
+      <c r="A28" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="57"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="57"/>
-      <c r="E28" s="57"/>
-      <c r="F28" s="57"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
@@ -26295,22 +26280,22 @@
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="58" t="s">
+      <c r="A34" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="B34" s="58"/>
-      <c r="C34" s="58"/>
-      <c r="D34" s="58"/>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
+      <c r="B34" s="63"/>
+      <c r="C34" s="63"/>
+      <c r="D34" s="63"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="63"/>
       <c r="G34" s="18"/>
-      <c r="I34" s="59" t="s">
+      <c r="I34" s="64" t="s">
         <v>166</v>
       </c>
-      <c r="J34" s="59"/>
-      <c r="K34" s="59"/>
-      <c r="L34" s="59"/>
-      <c r="M34" s="59"/>
+      <c r="J34" s="64"/>
+      <c r="K34" s="64"/>
+      <c r="L34" s="64"/>
+      <c r="M34" s="64"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
@@ -26331,11 +26316,11 @@
       <c r="F35" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="I35" s="59" t="s">
+      <c r="I35" s="64" t="s">
         <v>167</v>
       </c>
-      <c r="J35" s="59"/>
-      <c r="K35" s="59"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="64"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="18">
@@ -26359,13 +26344,13 @@
       <c r="G36" s="5">
         <v>0.27</v>
       </c>
-      <c r="I36" s="60" t="s">
+      <c r="I36" s="65" t="s">
         <v>170</v>
       </c>
-      <c r="J36" s="60"/>
-      <c r="K36" s="60"/>
-      <c r="L36" s="60"/>
-      <c r="M36" s="60"/>
+      <c r="J36" s="65"/>
+      <c r="K36" s="65"/>
+      <c r="L36" s="65"/>
+      <c r="M36" s="65"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="18">
@@ -26437,14 +26422,14 @@
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A40" s="58" t="s">
+      <c r="A40" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="58"/>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
-      <c r="E40" s="58"/>
-      <c r="F40" s="58"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="63"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="63"/>
+      <c r="F40" s="63"/>
       <c r="G40" s="18"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
@@ -26561,14 +26546,14 @@
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" s="58" t="s">
+      <c r="A46" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="B46" s="58"/>
-      <c r="C46" s="58"/>
-      <c r="D46" s="58"/>
-      <c r="E46" s="58"/>
-      <c r="F46" s="58"/>
+      <c r="B46" s="63"/>
+      <c r="C46" s="63"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="63"/>
+      <c r="F46" s="63"/>
       <c r="G46" s="18"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -26685,14 +26670,14 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" s="57" t="s">
+      <c r="A52" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="57"/>
-      <c r="C52" s="57"/>
-      <c r="D52" s="57"/>
-      <c r="E52" s="57"/>
-      <c r="F52" s="57"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="61"/>
       <c r="G52" s="7"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
@@ -26809,39 +26794,39 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="57" t="s">
+      <c r="A60" s="61" t="s">
         <v>106</v>
       </c>
-      <c r="B60" s="57"/>
-      <c r="C60" s="57"/>
-      <c r="D60" s="57"/>
-      <c r="E60" s="57"/>
-      <c r="F60" s="57"/>
-      <c r="G60" s="57"/>
-      <c r="H60" s="57"/>
-      <c r="I60" s="57"/>
-      <c r="J60" s="57"/>
-      <c r="K60" s="57"/>
+      <c r="B60" s="61"/>
+      <c r="C60" s="61"/>
+      <c r="D60" s="61"/>
+      <c r="E60" s="61"/>
+      <c r="F60" s="61"/>
+      <c r="G60" s="61"/>
+      <c r="H60" s="61"/>
+      <c r="I60" s="61"/>
+      <c r="J60" s="61"/>
+      <c r="K60" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="A28:F28"/>
+    <mergeCell ref="A34:F34"/>
+    <mergeCell ref="A40:F40"/>
+    <mergeCell ref="A46:F46"/>
+    <mergeCell ref="A52:F52"/>
+    <mergeCell ref="A60:K60"/>
+    <mergeCell ref="I34:M34"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="I36:M36"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A25:J25"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A46:F46"/>
-    <mergeCell ref="A52:F52"/>
-    <mergeCell ref="A60:K60"/>
-    <mergeCell ref="I34:M34"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="I36:M36"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="A28:F28"/>
-    <mergeCell ref="A34:F34"/>
-    <mergeCell ref="A40:F40"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -26866,19 +26851,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61"/>
       <c r="L1" s="7" t="s">
         <v>164</v>
       </c>
@@ -26899,19 +26884,19 @@
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
       <c r="L3" s="5"/>
       <c r="M3" s="23"/>
       <c r="N3" s="23"/>
@@ -26921,19 +26906,19 @@
       <c r="R3" s="23"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="58" t="s">
+      <c r="A4" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
       <c r="L4" s="21"/>
       <c r="M4" s="23"/>
       <c r="N4" s="23"/>
@@ -27068,19 +27053,19 @@
       <c r="R7" s="12"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="58" t="s">
+      <c r="A8" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="58"/>
-      <c r="I8" s="58"/>
-      <c r="J8" s="58"/>
-      <c r="K8" s="58"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="63"/>
+      <c r="K8" s="63"/>
       <c r="L8" s="5"/>
       <c r="M8" s="23"/>
       <c r="N8" s="23"/>
@@ -27216,19 +27201,19 @@
       <c r="R11" s="12"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="58" t="s">
+      <c r="A12" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
-      <c r="D12" s="58"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="58"/>
-      <c r="H12" s="58"/>
-      <c r="I12" s="58"/>
-      <c r="J12" s="58"/>
-      <c r="K12" s="58"/>
+      <c r="B12" s="63"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
       <c r="L12" s="18"/>
       <c r="M12" s="23"/>
       <c r="N12" s="23"/>
@@ -27367,38 +27352,38 @@
       <c r="L16" s="22"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="62" t="s">
+      <c r="A17" s="66" t="s">
         <v>197</v>
       </c>
-      <c r="B17" s="62"/>
-      <c r="C17" s="62"/>
-      <c r="D17" s="62"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
+      <c r="B17" s="66"/>
+      <c r="C17" s="66"/>
+      <c r="D17" s="66"/>
+      <c r="E17" s="66"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="66"/>
+      <c r="H17" s="66"/>
+      <c r="I17" s="66"/>
+      <c r="J17" s="66"/>
+      <c r="K17" s="66"/>
       <c r="L17" s="5"/>
       <c r="M17" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
       <c r="L18" s="5"/>
       <c r="M18" t="s">
         <v>272</v>
@@ -27513,19 +27498,19 @@
       <c r="L21" s="22"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="58" t="s">
+      <c r="A22" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B22" s="58"/>
-      <c r="C22" s="58"/>
-      <c r="D22" s="58"/>
-      <c r="E22" s="58"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="58"/>
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
-      <c r="J22" s="58"/>
-      <c r="K22" s="58"/>
+      <c r="B22" s="63"/>
+      <c r="C22" s="63"/>
+      <c r="D22" s="63"/>
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63"/>
+      <c r="H22" s="63"/>
+      <c r="I22" s="63"/>
+      <c r="J22" s="63"/>
+      <c r="K22" s="63"/>
       <c r="L22" s="7"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
@@ -27637,19 +27622,19 @@
       <c r="L25" s="22"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A26" s="58" t="s">
+      <c r="A26" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B26" s="58"/>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
-      <c r="J26" s="58"/>
-      <c r="K26" s="58"/>
+      <c r="B26" s="63"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="63"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="63"/>
+      <c r="K26" s="63"/>
       <c r="L26" s="22"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -27759,55 +27744,55 @@
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A30" s="57"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="57"/>
-      <c r="D30" s="57"/>
-      <c r="E30" s="57"/>
-      <c r="F30" s="57"/>
-      <c r="G30" s="57"/>
-      <c r="H30" s="57"/>
-      <c r="I30" s="57"/>
-      <c r="J30" s="57"/>
-      <c r="K30" s="57"/>
-      <c r="L30" s="57"/>
-      <c r="M30" s="57"/>
-      <c r="N30" s="57"/>
-      <c r="O30" s="57"/>
-      <c r="P30" s="57"/>
+      <c r="A30" s="61"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="61"/>
+      <c r="L30" s="61"/>
+      <c r="M30" s="61"/>
+      <c r="N30" s="61"/>
+      <c r="O30" s="61"/>
+      <c r="P30" s="61"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A32" s="62" t="s">
+      <c r="A32" s="66" t="s">
         <v>199</v>
       </c>
-      <c r="B32" s="62"/>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="62"/>
-      <c r="H32" s="62"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="62"/>
-      <c r="K32" s="62"/>
+      <c r="B32" s="66"/>
+      <c r="C32" s="66"/>
+      <c r="D32" s="66"/>
+      <c r="E32" s="66"/>
+      <c r="F32" s="66"/>
+      <c r="G32" s="66"/>
+      <c r="H32" s="66"/>
+      <c r="I32" s="66"/>
+      <c r="J32" s="66"/>
+      <c r="K32" s="66"/>
       <c r="M32" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="57" t="s">
+      <c r="A33" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="B33" s="57"/>
-      <c r="C33" s="57"/>
-      <c r="D33" s="57"/>
-      <c r="E33" s="57"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="57"/>
-      <c r="J33" s="57"/>
-      <c r="K33" s="57"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="61"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="19" t="s">
@@ -27915,19 +27900,19 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" s="58" t="s">
+      <c r="A37" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="58"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="58"/>
+      <c r="B37" s="63"/>
+      <c r="C37" s="63"/>
+      <c r="D37" s="63"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="63"/>
+      <c r="H37" s="63"/>
+      <c r="I37" s="63"/>
+      <c r="J37" s="63"/>
+      <c r="K37" s="63"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
@@ -28035,19 +28020,19 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" s="58" t="s">
+      <c r="A41" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B41" s="58"/>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
-      <c r="J41" s="58"/>
-      <c r="K41" s="58"/>
+      <c r="B41" s="63"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="63"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="63"/>
+      <c r="H41" s="63"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="63"/>
+      <c r="K41" s="63"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
@@ -28173,34 +28158,34 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="62" t="s">
+      <c r="A49" s="66" t="s">
         <v>182</v>
       </c>
-      <c r="B49" s="62"/>
-      <c r="C49" s="62"/>
-      <c r="D49" s="62"/>
-      <c r="E49" s="62"/>
-      <c r="F49" s="62"/>
-      <c r="G49" s="62"/>
-      <c r="H49" s="62"/>
-      <c r="I49" s="62"/>
-      <c r="J49" s="62"/>
-      <c r="K49" s="62"/>
+      <c r="B49" s="66"/>
+      <c r="C49" s="66"/>
+      <c r="D49" s="66"/>
+      <c r="E49" s="66"/>
+      <c r="F49" s="66"/>
+      <c r="G49" s="66"/>
+      <c r="H49" s="66"/>
+      <c r="I49" s="66"/>
+      <c r="J49" s="66"/>
+      <c r="K49" s="66"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="58" t="s">
+      <c r="A50" s="63" t="s">
         <v>100</v>
       </c>
-      <c r="B50" s="58"/>
-      <c r="C50" s="58"/>
-      <c r="D50" s="58"/>
-      <c r="E50" s="58"/>
-      <c r="F50" s="58"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-      <c r="J50" s="58"/>
-      <c r="K50" s="58"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="63"/>
+      <c r="D50" s="63"/>
+      <c r="E50" s="63"/>
+      <c r="F50" s="63"/>
+      <c r="G50" s="63"/>
+      <c r="H50" s="63"/>
+      <c r="I50" s="63"/>
+      <c r="J50" s="63"/>
+      <c r="K50" s="63"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
@@ -28308,19 +28293,19 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" s="58" t="s">
+      <c r="A54" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B54" s="58"/>
-      <c r="C54" s="58"/>
-      <c r="D54" s="58"/>
-      <c r="E54" s="58"/>
-      <c r="F54" s="58"/>
-      <c r="G54" s="58"/>
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
-      <c r="J54" s="58"/>
-      <c r="K54" s="58"/>
+      <c r="B54" s="63"/>
+      <c r="C54" s="63"/>
+      <c r="D54" s="63"/>
+      <c r="E54" s="63"/>
+      <c r="F54" s="63"/>
+      <c r="G54" s="63"/>
+      <c r="H54" s="63"/>
+      <c r="I54" s="63"/>
+      <c r="J54" s="63"/>
+      <c r="K54" s="63"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="18" t="s">
@@ -28428,19 +28413,19 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="58" t="s">
+      <c r="A58" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B58" s="58"/>
-      <c r="C58" s="58"/>
-      <c r="D58" s="58"/>
-      <c r="E58" s="58"/>
-      <c r="F58" s="58"/>
-      <c r="G58" s="58"/>
-      <c r="H58" s="58"/>
-      <c r="I58" s="58"/>
-      <c r="J58" s="58"/>
-      <c r="K58" s="58"/>
+      <c r="B58" s="63"/>
+      <c r="C58" s="63"/>
+      <c r="D58" s="63"/>
+      <c r="E58" s="63"/>
+      <c r="F58" s="63"/>
+      <c r="G58" s="63"/>
+      <c r="H58" s="63"/>
+      <c r="I58" s="63"/>
+      <c r="J58" s="63"/>
+      <c r="K58" s="63"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="18" t="s">
@@ -28548,34 +28533,34 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="62" t="s">
+      <c r="A63" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="B63" s="62"/>
-      <c r="C63" s="62"/>
-      <c r="D63" s="62"/>
-      <c r="E63" s="62"/>
-      <c r="F63" s="62"/>
-      <c r="G63" s="62"/>
-      <c r="H63" s="62"/>
-      <c r="I63" s="62"/>
-      <c r="J63" s="62"/>
-      <c r="K63" s="62"/>
+      <c r="B63" s="66"/>
+      <c r="C63" s="66"/>
+      <c r="D63" s="66"/>
+      <c r="E63" s="66"/>
+      <c r="F63" s="66"/>
+      <c r="G63" s="66"/>
+      <c r="H63" s="66"/>
+      <c r="I63" s="66"/>
+      <c r="J63" s="66"/>
+      <c r="K63" s="66"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="57" t="s">
+      <c r="A64" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="B64" s="57"/>
-      <c r="C64" s="57"/>
-      <c r="D64" s="57"/>
-      <c r="E64" s="57"/>
-      <c r="F64" s="57"/>
-      <c r="G64" s="57"/>
-      <c r="H64" s="57"/>
-      <c r="I64" s="57"/>
-      <c r="J64" s="57"/>
-      <c r="K64" s="57"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="61"/>
+      <c r="D64" s="61"/>
+      <c r="E64" s="61"/>
+      <c r="F64" s="61"/>
+      <c r="G64" s="61"/>
+      <c r="H64" s="61"/>
+      <c r="I64" s="61"/>
+      <c r="J64" s="61"/>
+      <c r="K64" s="61"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="18" t="s">
@@ -28683,19 +28668,19 @@
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="58" t="s">
+      <c r="A68" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B68" s="58"/>
-      <c r="C68" s="58"/>
-      <c r="D68" s="58"/>
-      <c r="E68" s="58"/>
-      <c r="F68" s="58"/>
-      <c r="G68" s="58"/>
-      <c r="H68" s="58"/>
-      <c r="I68" s="58"/>
-      <c r="J68" s="58"/>
-      <c r="K68" s="58"/>
+      <c r="B68" s="63"/>
+      <c r="C68" s="63"/>
+      <c r="D68" s="63"/>
+      <c r="E68" s="63"/>
+      <c r="F68" s="63"/>
+      <c r="G68" s="63"/>
+      <c r="H68" s="63"/>
+      <c r="I68" s="63"/>
+      <c r="J68" s="63"/>
+      <c r="K68" s="63"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="18" t="s">
@@ -28803,19 +28788,19 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="58" t="s">
+      <c r="A72" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B72" s="58"/>
-      <c r="C72" s="58"/>
-      <c r="D72" s="58"/>
-      <c r="E72" s="58"/>
-      <c r="F72" s="58"/>
-      <c r="G72" s="58"/>
-      <c r="H72" s="58"/>
-      <c r="I72" s="58"/>
-      <c r="J72" s="58"/>
-      <c r="K72" s="58"/>
+      <c r="B72" s="63"/>
+      <c r="C72" s="63"/>
+      <c r="D72" s="63"/>
+      <c r="E72" s="63"/>
+      <c r="F72" s="63"/>
+      <c r="G72" s="63"/>
+      <c r="H72" s="63"/>
+      <c r="I72" s="63"/>
+      <c r="J72" s="63"/>
+      <c r="K72" s="63"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="18" t="s">
@@ -28923,34 +28908,34 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="62" t="s">
+      <c r="A78" s="66" t="s">
         <v>196</v>
       </c>
-      <c r="B78" s="62"/>
-      <c r="C78" s="62"/>
-      <c r="D78" s="62"/>
-      <c r="E78" s="62"/>
-      <c r="F78" s="62"/>
-      <c r="G78" s="62"/>
-      <c r="H78" s="62"/>
-      <c r="I78" s="62"/>
-      <c r="J78" s="62"/>
-      <c r="K78" s="62"/>
+      <c r="B78" s="66"/>
+      <c r="C78" s="66"/>
+      <c r="D78" s="66"/>
+      <c r="E78" s="66"/>
+      <c r="F78" s="66"/>
+      <c r="G78" s="66"/>
+      <c r="H78" s="66"/>
+      <c r="I78" s="66"/>
+      <c r="J78" s="66"/>
+      <c r="K78" s="66"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" s="57" t="s">
+      <c r="A79" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="B79" s="57"/>
-      <c r="C79" s="57"/>
-      <c r="D79" s="57"/>
-      <c r="E79" s="57"/>
-      <c r="F79" s="57"/>
-      <c r="G79" s="57"/>
-      <c r="H79" s="57"/>
-      <c r="I79" s="57"/>
-      <c r="J79" s="57"/>
-      <c r="K79" s="57"/>
+      <c r="B79" s="61"/>
+      <c r="C79" s="61"/>
+      <c r="D79" s="61"/>
+      <c r="E79" s="61"/>
+      <c r="F79" s="61"/>
+      <c r="G79" s="61"/>
+      <c r="H79" s="61"/>
+      <c r="I79" s="61"/>
+      <c r="J79" s="61"/>
+      <c r="K79" s="61"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="19" t="s">
@@ -29058,19 +29043,19 @@
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="58" t="s">
+      <c r="A83" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B83" s="58"/>
-      <c r="C83" s="58"/>
-      <c r="D83" s="58"/>
-      <c r="E83" s="58"/>
-      <c r="F83" s="58"/>
-      <c r="G83" s="58"/>
-      <c r="H83" s="58"/>
-      <c r="I83" s="58"/>
-      <c r="J83" s="58"/>
-      <c r="K83" s="58"/>
+      <c r="B83" s="63"/>
+      <c r="C83" s="63"/>
+      <c r="D83" s="63"/>
+      <c r="E83" s="63"/>
+      <c r="F83" s="63"/>
+      <c r="G83" s="63"/>
+      <c r="H83" s="63"/>
+      <c r="I83" s="63"/>
+      <c r="J83" s="63"/>
+      <c r="K83" s="63"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="19" t="s">
@@ -29178,19 +29163,19 @@
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="58" t="s">
+      <c r="A87" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B87" s="58"/>
-      <c r="C87" s="58"/>
-      <c r="D87" s="58"/>
-      <c r="E87" s="58"/>
-      <c r="F87" s="58"/>
-      <c r="G87" s="58"/>
-      <c r="H87" s="58"/>
-      <c r="I87" s="58"/>
-      <c r="J87" s="58"/>
-      <c r="K87" s="58"/>
+      <c r="B87" s="63"/>
+      <c r="C87" s="63"/>
+      <c r="D87" s="63"/>
+      <c r="E87" s="63"/>
+      <c r="F87" s="63"/>
+      <c r="G87" s="63"/>
+      <c r="H87" s="63"/>
+      <c r="I87" s="63"/>
+      <c r="J87" s="63"/>
+      <c r="K87" s="63"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="19" t="s">
@@ -29324,34 +29309,34 @@
       <c r="K92" s="24"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A93" s="62" t="s">
+      <c r="A93" s="66" t="s">
         <v>199</v>
       </c>
-      <c r="B93" s="62"/>
-      <c r="C93" s="62"/>
-      <c r="D93" s="62"/>
-      <c r="E93" s="62"/>
-      <c r="F93" s="62"/>
-      <c r="G93" s="62"/>
-      <c r="H93" s="62"/>
-      <c r="I93" s="62"/>
-      <c r="J93" s="62"/>
-      <c r="K93" s="62"/>
+      <c r="B93" s="66"/>
+      <c r="C93" s="66"/>
+      <c r="D93" s="66"/>
+      <c r="E93" s="66"/>
+      <c r="F93" s="66"/>
+      <c r="G93" s="66"/>
+      <c r="H93" s="66"/>
+      <c r="I93" s="66"/>
+      <c r="J93" s="66"/>
+      <c r="K93" s="66"/>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A94" s="57" t="s">
+      <c r="A94" s="61" t="s">
         <v>100</v>
       </c>
-      <c r="B94" s="57"/>
-      <c r="C94" s="57"/>
-      <c r="D94" s="57"/>
-      <c r="E94" s="57"/>
-      <c r="F94" s="57"/>
-      <c r="G94" s="57"/>
-      <c r="H94" s="57"/>
-      <c r="I94" s="57"/>
-      <c r="J94" s="57"/>
-      <c r="K94" s="57"/>
+      <c r="B94" s="61"/>
+      <c r="C94" s="61"/>
+      <c r="D94" s="61"/>
+      <c r="E94" s="61"/>
+      <c r="F94" s="61"/>
+      <c r="G94" s="61"/>
+      <c r="H94" s="61"/>
+      <c r="I94" s="61"/>
+      <c r="J94" s="61"/>
+      <c r="K94" s="61"/>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="27" t="s">
@@ -29459,19 +29444,19 @@
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A98" s="58" t="s">
+      <c r="A98" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="B98" s="58"/>
-      <c r="C98" s="58"/>
-      <c r="D98" s="58"/>
-      <c r="E98" s="58"/>
-      <c r="F98" s="58"/>
-      <c r="G98" s="58"/>
-      <c r="H98" s="58"/>
-      <c r="I98" s="58"/>
-      <c r="J98" s="58"/>
-      <c r="K98" s="58"/>
+      <c r="B98" s="63"/>
+      <c r="C98" s="63"/>
+      <c r="D98" s="63"/>
+      <c r="E98" s="63"/>
+      <c r="F98" s="63"/>
+      <c r="G98" s="63"/>
+      <c r="H98" s="63"/>
+      <c r="I98" s="63"/>
+      <c r="J98" s="63"/>
+      <c r="K98" s="63"/>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="27" t="s">
@@ -29579,19 +29564,19 @@
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A102" s="58" t="s">
+      <c r="A102" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="B102" s="58"/>
-      <c r="C102" s="58"/>
-      <c r="D102" s="58"/>
-      <c r="E102" s="58"/>
-      <c r="F102" s="58"/>
-      <c r="G102" s="58"/>
-      <c r="H102" s="58"/>
-      <c r="I102" s="58"/>
-      <c r="J102" s="58"/>
-      <c r="K102" s="58"/>
+      <c r="B102" s="63"/>
+      <c r="C102" s="63"/>
+      <c r="D102" s="63"/>
+      <c r="E102" s="63"/>
+      <c r="F102" s="63"/>
+      <c r="G102" s="63"/>
+      <c r="H102" s="63"/>
+      <c r="I102" s="63"/>
+      <c r="J102" s="63"/>
+      <c r="K102" s="63"/>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="27" t="s">
@@ -29700,6 +29685,20 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="A93:K93"/>
+    <mergeCell ref="A94:K94"/>
+    <mergeCell ref="A98:K98"/>
+    <mergeCell ref="A102:K102"/>
+    <mergeCell ref="A54:K54"/>
+    <mergeCell ref="A58:K58"/>
+    <mergeCell ref="A63:K63"/>
+    <mergeCell ref="A64:K64"/>
+    <mergeCell ref="A68:K68"/>
+    <mergeCell ref="A72:K72"/>
+    <mergeCell ref="A78:K78"/>
+    <mergeCell ref="A79:K79"/>
+    <mergeCell ref="A83:K83"/>
+    <mergeCell ref="A87:K87"/>
     <mergeCell ref="A50:K50"/>
     <mergeCell ref="A30:P30"/>
     <mergeCell ref="A12:K12"/>
@@ -29716,20 +29715,6 @@
     <mergeCell ref="A22:K22"/>
     <mergeCell ref="A26:K26"/>
     <mergeCell ref="A49:K49"/>
-    <mergeCell ref="A93:K93"/>
-    <mergeCell ref="A94:K94"/>
-    <mergeCell ref="A98:K98"/>
-    <mergeCell ref="A102:K102"/>
-    <mergeCell ref="A54:K54"/>
-    <mergeCell ref="A58:K58"/>
-    <mergeCell ref="A63:K63"/>
-    <mergeCell ref="A64:K64"/>
-    <mergeCell ref="A68:K68"/>
-    <mergeCell ref="A72:K72"/>
-    <mergeCell ref="A78:K78"/>
-    <mergeCell ref="A79:K79"/>
-    <mergeCell ref="A83:K83"/>
-    <mergeCell ref="A87:K87"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -29742,7 +29727,7 @@
   <dimension ref="A2:DE48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N44" sqref="N44"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29762,56 +29747,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="61" t="s">
         <v>64</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="H2" s="57" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="H2" s="61" t="s">
         <v>526</v>
       </c>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="O2" s="61" t="s">
         <v>358</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="H3" s="66" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="H3" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="O3" s="66" t="s">
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="O3" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
     </row>
     <row r="4" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -30094,30 +30079,30 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="57" t="s">
+      <c r="A9" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="H9" s="57" t="s">
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+      <c r="H9" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="57"/>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="57"/>
-      <c r="O9" s="57" t="s">
+      <c r="I9" s="61"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="61"/>
+      <c r="L9" s="61"/>
+      <c r="M9" s="61"/>
+      <c r="O9" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="P9" s="57"/>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="61"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -30229,7 +30214,7 @@
       <c r="S11" s="44" t="s">
         <v>309</v>
       </c>
-      <c r="T11" s="71" t="s">
+      <c r="T11" s="57" t="s">
         <v>301</v>
       </c>
     </row>
@@ -30286,7 +30271,7 @@
       <c r="S12" s="44" t="s">
         <v>310</v>
       </c>
-      <c r="T12" s="71" t="s">
+      <c r="T12" s="57" t="s">
         <v>302</v>
       </c>
     </row>
@@ -30343,7 +30328,7 @@
       <c r="S13" s="44" t="s">
         <v>311</v>
       </c>
-      <c r="T13" s="71" t="s">
+      <c r="T13" s="57" t="s">
         <v>303</v>
       </c>
     </row>
@@ -30400,36 +30385,36 @@
       <c r="S14" s="44" t="s">
         <v>312</v>
       </c>
-      <c r="T14" s="71" t="s">
+      <c r="T14" s="57" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="63" t="s">
         <v>274</v>
       </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="H15" s="58" t="s">
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="H15" s="63" t="s">
         <v>274</v>
       </c>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="58"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
       <c r="N15" s="12"/>
-      <c r="O15" s="58" t="s">
+      <c r="O15" s="63" t="s">
         <v>274</v>
       </c>
-      <c r="P15" s="58"/>
-      <c r="Q15" s="58"/>
-      <c r="R15" s="58"/>
-      <c r="S15" s="58"/>
-      <c r="T15" s="58"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="63"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="63"/>
+      <c r="T15" s="63"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="41" t="s">
@@ -30732,48 +30717,48 @@
       <c r="T21" s="12"/>
     </row>
     <row r="23" spans="1:109" x14ac:dyDescent="0.25">
-      <c r="A23" s="57"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
     </row>
     <row r="24" spans="1:109" x14ac:dyDescent="0.25">
-      <c r="A24" s="57"/>
-      <c r="B24" s="57"/>
-      <c r="C24" s="57"/>
-      <c r="D24" s="57"/>
-      <c r="E24" s="57"/>
-      <c r="F24" s="57"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
     </row>
     <row r="25" spans="1:109" x14ac:dyDescent="0.25">
-      <c r="A25" s="65" t="s">
+      <c r="A25" s="70" t="s">
         <v>277</v>
       </c>
-      <c r="B25" s="65"/>
-      <c r="C25" s="65"/>
-      <c r="D25" s="65"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="65"/>
-      <c r="H25" s="64" t="s">
+      <c r="B25" s="70"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="70"/>
+      <c r="F25" s="70"/>
+      <c r="H25" s="69" t="s">
         <v>384</v>
       </c>
-      <c r="I25" s="64"/>
-      <c r="J25" s="64"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="64"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="69"/>
     </row>
     <row r="26" spans="1:109" x14ac:dyDescent="0.25">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="57"/>
-      <c r="C26" s="57"/>
-      <c r="D26" s="57"/>
-      <c r="E26" s="57"/>
-      <c r="F26" s="57"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
     </row>
     <row r="27" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
@@ -30794,7 +30779,7 @@
       <c r="F27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H27" s="63" t="s">
+      <c r="H27" s="68" t="s">
         <v>278</v>
       </c>
       <c r="I27" t="s">
@@ -30830,7 +30815,7 @@
       <c r="F28">
         <v>18272</v>
       </c>
-      <c r="H28" s="63"/>
+      <c r="H28" s="68"/>
       <c r="I28" t="s">
         <v>5</v>
       </c>
@@ -31154,7 +31139,7 @@
       <c r="F29">
         <v>18191</v>
       </c>
-      <c r="H29" s="63"/>
+      <c r="H29" s="68"/>
       <c r="I29" t="s">
         <v>6</v>
       </c>
@@ -31511,15 +31496,15 @@
       <c r="M31" s="23"/>
     </row>
     <row r="32" spans="1:109" x14ac:dyDescent="0.25">
-      <c r="A32" s="57" t="s">
+      <c r="A32" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="57"/>
-      <c r="C32" s="57"/>
-      <c r="D32" s="57"/>
-      <c r="E32" s="57"/>
-      <c r="F32" s="57"/>
-      <c r="H32" s="63" t="s">
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="H32" s="68" t="s">
         <v>280</v>
       </c>
       <c r="I32" t="s">
@@ -31555,7 +31540,7 @@
       <c r="F33" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H33" s="63"/>
+      <c r="H33" s="68"/>
       <c r="I33" t="s">
         <v>5</v>
       </c>
@@ -31879,7 +31864,7 @@
       <c r="F34">
         <v>18326</v>
       </c>
-      <c r="H34" s="63"/>
+      <c r="H34" s="68"/>
       <c r="I34" t="s">
         <v>6</v>
       </c>
@@ -32247,7 +32232,7 @@
       <c r="F37">
         <v>19001</v>
       </c>
-      <c r="H37" s="63" t="s">
+      <c r="H37" s="68" t="s">
         <v>281</v>
       </c>
       <c r="I37" t="s">
@@ -32270,15 +32255,15 @@
       </c>
     </row>
     <row r="38" spans="1:109" x14ac:dyDescent="0.25">
-      <c r="A38" s="57" t="s">
+      <c r="A38" s="61" t="s">
         <v>274</v>
       </c>
-      <c r="B38" s="57"/>
-      <c r="C38" s="57"/>
-      <c r="D38" s="57"/>
-      <c r="E38" s="57"/>
-      <c r="F38" s="57"/>
-      <c r="H38" s="63"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="61"/>
+      <c r="E38" s="61"/>
+      <c r="F38" s="61"/>
+      <c r="H38" s="68"/>
       <c r="I38" t="s">
         <v>5</v>
       </c>
@@ -32602,7 +32587,7 @@
       <c r="F39" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H39" s="63"/>
+      <c r="H39" s="68"/>
       <c r="I39" t="s">
         <v>6</v>
       </c>
@@ -32948,7 +32933,7 @@
       <c r="F41">
         <v>18299</v>
       </c>
-      <c r="H41" s="63" t="s">
+      <c r="H41" s="68" t="s">
         <v>282</v>
       </c>
       <c r="I41" t="s">
@@ -32984,7 +32969,7 @@
       <c r="F42">
         <v>19163</v>
       </c>
-      <c r="H42" s="63"/>
+      <c r="H42" s="68"/>
       <c r="I42" t="s">
         <v>5</v>
       </c>
@@ -33308,7 +33293,7 @@
       <c r="F43">
         <v>19055</v>
       </c>
-      <c r="H43" s="63"/>
+      <c r="H43" s="68"/>
       <c r="I43" t="s">
         <v>6</v>
       </c>
@@ -33646,6 +33631,20 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="H41:H43"/>
+    <mergeCell ref="H25:M25"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A26:F26"/>
+    <mergeCell ref="H27:H29"/>
+    <mergeCell ref="H32:H34"/>
+    <mergeCell ref="H37:H39"/>
+    <mergeCell ref="A32:F32"/>
+    <mergeCell ref="A38:F38"/>
+    <mergeCell ref="O2:T2"/>
+    <mergeCell ref="O3:T3"/>
+    <mergeCell ref="O9:T9"/>
+    <mergeCell ref="O15:T15"/>
+    <mergeCell ref="H3:M3"/>
     <mergeCell ref="A24:F24"/>
     <mergeCell ref="A23:F23"/>
     <mergeCell ref="A9:F9"/>
@@ -33655,20 +33654,6 @@
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="A3:F3"/>
     <mergeCell ref="H15:M15"/>
-    <mergeCell ref="O2:T2"/>
-    <mergeCell ref="O3:T3"/>
-    <mergeCell ref="O9:T9"/>
-    <mergeCell ref="O15:T15"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="H41:H43"/>
-    <mergeCell ref="H25:M25"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A26:F26"/>
-    <mergeCell ref="H27:H29"/>
-    <mergeCell ref="H32:H34"/>
-    <mergeCell ref="H37:H39"/>
-    <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A38:F38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -33681,7 +33666,7 @@
   <dimension ref="A2:BG42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O49" sqref="O49"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33700,56 +33685,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="61" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="H2" s="57" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="H2" s="61" t="s">
         <v>526</v>
       </c>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="O2" s="61" t="s">
         <v>358</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="H3" s="66" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="H3" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="O3" s="66" t="s">
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="O3" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
     </row>
     <row r="4" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -34032,30 +34017,30 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="H9" s="58" t="s">
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="H9" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="O9" s="57" t="s">
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="O9" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="P9" s="57"/>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="61"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -34338,30 +34323,30 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="63" t="s">
         <v>274</v>
       </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="H15" s="58" t="s">
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="H15" s="63" t="s">
         <v>274</v>
       </c>
-      <c r="I15" s="58"/>
-      <c r="J15" s="58"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="58"/>
-      <c r="M15" s="58"/>
-      <c r="O15" s="67" t="s">
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="K15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15" s="63"/>
+      <c r="O15" s="71" t="s">
         <v>274</v>
       </c>
-      <c r="P15" s="67"/>
-      <c r="Q15" s="67"/>
-      <c r="R15" s="67"/>
-      <c r="S15" s="67"/>
-      <c r="T15" s="67"/>
+      <c r="P15" s="71"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="71"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="71"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
@@ -34644,40 +34629,40 @@
       </c>
     </row>
     <row r="23" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A23" s="57"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
     </row>
     <row r="24" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="70" t="s">
         <v>277</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="H24" s="64" t="s">
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="H24" s="69" t="s">
         <v>384</v>
       </c>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
     </row>
     <row r="25" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
     </row>
     <row r="26" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A26" s="42" t="s">
@@ -34698,7 +34683,7 @@
       <c r="F26" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="63" t="s">
+      <c r="H26" s="68" t="s">
         <v>278</v>
       </c>
       <c r="I26" t="s">
@@ -34730,7 +34715,7 @@
       <c r="F27">
         <v>18272</v>
       </c>
-      <c r="H27" s="63"/>
+      <c r="H27" s="68"/>
       <c r="I27" t="s">
         <v>5</v>
       </c>
@@ -34904,7 +34889,7 @@
       <c r="F28">
         <v>18191</v>
       </c>
-      <c r="H28" s="63"/>
+      <c r="H28" s="68"/>
       <c r="I28" t="s">
         <v>6</v>
       </c>
@@ -35102,15 +35087,15 @@
       <c r="H30" s="23"/>
     </row>
     <row r="31" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="H31" s="63" t="s">
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="H31" s="68" t="s">
         <v>280</v>
       </c>
       <c r="I31" t="s">
@@ -35142,7 +35127,7 @@
       <c r="F32" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="H32" s="63"/>
+      <c r="H32" s="68"/>
       <c r="I32" t="s">
         <v>5</v>
       </c>
@@ -35316,7 +35301,7 @@
       <c r="F33">
         <v>18326</v>
       </c>
-      <c r="H33" s="63"/>
+      <c r="H33" s="68"/>
       <c r="I33" t="s">
         <v>6</v>
       </c>
@@ -35532,7 +35517,7 @@
       <c r="F36">
         <v>19001</v>
       </c>
-      <c r="H36" s="63" t="s">
+      <c r="H36" s="68" t="s">
         <v>281</v>
       </c>
       <c r="I36" t="s">
@@ -35546,15 +35531,15 @@
       </c>
     </row>
     <row r="37" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A37" s="57" t="s">
+      <c r="A37" s="61" t="s">
         <v>274</v>
       </c>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="H37" s="63"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="H37" s="68"/>
       <c r="I37" t="s">
         <v>5</v>
       </c>
@@ -35728,7 +35713,7 @@
       <c r="F38" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="H38" s="63"/>
+      <c r="H38" s="68"/>
       <c r="I38" t="s">
         <v>6</v>
       </c>
@@ -35923,7 +35908,7 @@
       <c r="F40">
         <v>18299</v>
       </c>
-      <c r="H40" s="63" t="s">
+      <c r="H40" s="68" t="s">
         <v>282</v>
       </c>
       <c r="I40" t="s">
@@ -35955,7 +35940,7 @@
       <c r="F41">
         <v>19163</v>
       </c>
-      <c r="H41" s="63"/>
+      <c r="H41" s="68"/>
       <c r="I41" t="s">
         <v>5</v>
       </c>
@@ -36129,7 +36114,7 @@
       <c r="F42">
         <v>19055</v>
       </c>
-      <c r="H42" s="63"/>
+      <c r="H42" s="68"/>
       <c r="I42" t="s">
         <v>6</v>
       </c>
@@ -36286,6 +36271,16 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="H24:M24"/>
+    <mergeCell ref="H26:H28"/>
+    <mergeCell ref="H31:H33"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="H40:H42"/>
+    <mergeCell ref="A24:F24"/>
+    <mergeCell ref="A25:F25"/>
+    <mergeCell ref="A31:F31"/>
+    <mergeCell ref="A37:F37"/>
+    <mergeCell ref="A23:F23"/>
     <mergeCell ref="A15:F15"/>
     <mergeCell ref="H15:M15"/>
     <mergeCell ref="O2:T2"/>
@@ -36298,16 +36293,6 @@
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="A9:F9"/>
     <mergeCell ref="H9:M9"/>
-    <mergeCell ref="A24:F24"/>
-    <mergeCell ref="A25:F25"/>
-    <mergeCell ref="A31:F31"/>
-    <mergeCell ref="A37:F37"/>
-    <mergeCell ref="A23:F23"/>
-    <mergeCell ref="H24:M24"/>
-    <mergeCell ref="H26:H28"/>
-    <mergeCell ref="H31:H33"/>
-    <mergeCell ref="H36:H38"/>
-    <mergeCell ref="H40:H42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -36319,8 +36304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:DE42"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36339,56 +36324,56 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="57" t="s">
+      <c r="A2" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="H2" s="57" t="s">
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="H2" s="61" t="s">
         <v>526</v>
       </c>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="57"/>
-      <c r="O2" s="57" t="s">
+      <c r="I2" s="61"/>
+      <c r="J2" s="61"/>
+      <c r="K2" s="61"/>
+      <c r="L2" s="61"/>
+      <c r="M2" s="61"/>
+      <c r="O2" s="61" t="s">
         <v>358</v>
       </c>
-      <c r="P2" s="57"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="57"/>
-      <c r="S2" s="57"/>
-      <c r="T2" s="57"/>
+      <c r="P2" s="61"/>
+      <c r="Q2" s="61"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="61"/>
+      <c r="T2" s="61"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="B3" s="57"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="H3" s="66" t="s">
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="H3" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="O3" s="66" t="s">
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="O3" s="67" t="s">
         <v>72</v>
       </c>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
     </row>
     <row r="4" spans="1:20" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
@@ -36468,19 +36453,19 @@
       <c r="H5" s="48">
         <v>0.1</v>
       </c>
-      <c r="I5" s="72">
+      <c r="I5" s="58">
         <v>645.25070000000005</v>
       </c>
-      <c r="J5" s="72">
+      <c r="J5" s="58">
         <v>1117.6256000000001</v>
       </c>
-      <c r="K5" s="72">
+      <c r="K5" s="58">
         <v>1504.0892000000001</v>
       </c>
-      <c r="L5" s="72">
+      <c r="L5" s="58">
         <v>1838.7799</v>
       </c>
-      <c r="M5" s="72">
+      <c r="M5" s="58">
         <v>1835.0492000000002</v>
       </c>
       <c r="O5" s="38">
@@ -36524,19 +36509,19 @@
       <c r="H6" s="48">
         <v>0.3</v>
       </c>
-      <c r="I6" s="72">
+      <c r="I6" s="58">
         <v>793.40880000000004</v>
       </c>
-      <c r="J6" s="72">
+      <c r="J6" s="58">
         <v>1100.0294000000001</v>
       </c>
-      <c r="K6" s="72">
+      <c r="K6" s="58">
         <v>1197.0563</v>
       </c>
-      <c r="L6" s="72">
+      <c r="L6" s="58">
         <v>1181.0839999999998</v>
       </c>
-      <c r="M6" s="72">
+      <c r="M6" s="58">
         <v>1108.502</v>
       </c>
       <c r="O6" s="38">
@@ -36580,19 +36565,19 @@
       <c r="H7" s="48">
         <v>0.5</v>
       </c>
-      <c r="I7" s="72">
+      <c r="I7" s="58">
         <v>829.74300000000005</v>
       </c>
-      <c r="J7" s="72">
+      <c r="J7" s="58">
         <v>1300.9973</v>
       </c>
-      <c r="K7" s="72">
+      <c r="K7" s="58">
         <v>1675.6378</v>
       </c>
-      <c r="L7" s="72">
+      <c r="L7" s="58">
         <v>1626.3543</v>
       </c>
-      <c r="M7" s="72">
+      <c r="M7" s="58">
         <v>1657.8720999999998</v>
       </c>
       <c r="O7" s="38">
@@ -36636,19 +36621,19 @@
       <c r="H8" s="48">
         <v>0.7</v>
       </c>
-      <c r="I8" s="72">
+      <c r="I8" s="58">
         <v>889.75979999999993</v>
       </c>
-      <c r="J8" s="72">
+      <c r="J8" s="58">
         <v>1536.3535999999999</v>
       </c>
-      <c r="K8" s="72">
+      <c r="K8" s="58">
         <v>1563.3735000000001</v>
       </c>
-      <c r="L8" s="72">
+      <c r="L8" s="58">
         <v>2056.2105999999999</v>
       </c>
-      <c r="M8" s="72">
+      <c r="M8" s="58">
         <v>1548.191</v>
       </c>
       <c r="O8" s="38">
@@ -36671,30 +36656,30 @@
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="58" t="s">
+      <c r="A9" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
-      <c r="D9" s="58"/>
-      <c r="E9" s="58"/>
-      <c r="F9" s="58"/>
-      <c r="H9" s="58" t="s">
+      <c r="B9" s="63"/>
+      <c r="C9" s="63"/>
+      <c r="D9" s="63"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63"/>
+      <c r="H9" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="I9" s="58"/>
-      <c r="J9" s="58"/>
-      <c r="K9" s="58"/>
-      <c r="L9" s="58"/>
-      <c r="M9" s="58"/>
-      <c r="O9" s="57" t="s">
+      <c r="I9" s="63"/>
+      <c r="J9" s="63"/>
+      <c r="K9" s="63"/>
+      <c r="L9" s="63"/>
+      <c r="M9" s="63"/>
+      <c r="O9" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="P9" s="57"/>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="57"/>
-      <c r="T9" s="57"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="61"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="61"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
@@ -36774,19 +36759,19 @@
       <c r="H11" s="22">
         <v>0.1</v>
       </c>
-      <c r="I11" s="73">
+      <c r="I11" s="59">
         <v>1430.0718999999999</v>
       </c>
-      <c r="J11" s="73">
+      <c r="J11" s="59">
         <v>1640.5157000000002</v>
       </c>
-      <c r="K11" s="73">
+      <c r="K11" s="59">
         <v>1619.9054000000001</v>
       </c>
-      <c r="L11" s="73">
+      <c r="L11" s="59">
         <v>2003.7892999999999</v>
       </c>
-      <c r="M11" s="73">
+      <c r="M11" s="59">
         <v>1835.0491</v>
       </c>
       <c r="N11" s="15"/>
@@ -36831,19 +36816,19 @@
       <c r="H12" s="22">
         <v>0.3</v>
       </c>
-      <c r="I12" s="73">
+      <c r="I12" s="59">
         <v>1342.2563</v>
       </c>
-      <c r="J12" s="73">
+      <c r="J12" s="59">
         <v>1486.2110999999998</v>
       </c>
-      <c r="K12" s="73">
+      <c r="K12" s="59">
         <v>1278.761</v>
       </c>
-      <c r="L12" s="73">
+      <c r="L12" s="59">
         <v>1190.7417</v>
       </c>
-      <c r="M12" s="73">
+      <c r="M12" s="59">
         <v>1108.5019</v>
       </c>
       <c r="N12" s="15"/>
@@ -36888,19 +36873,19 @@
       <c r="H13" s="22">
         <v>0.5</v>
       </c>
-      <c r="I13" s="73">
+      <c r="I13" s="59">
         <v>1577.7204000000002</v>
       </c>
-      <c r="J13" s="73">
+      <c r="J13" s="59">
         <v>1867.5438000000001</v>
       </c>
-      <c r="K13" s="73">
+      <c r="K13" s="59">
         <v>2041.7557999999999</v>
       </c>
-      <c r="L13" s="73">
+      <c r="L13" s="59">
         <v>1868.7972</v>
       </c>
-      <c r="M13" s="73">
+      <c r="M13" s="59">
         <v>1657.8720000000001</v>
       </c>
       <c r="N13" s="15"/>
@@ -36946,19 +36931,19 @@
       <c r="H14" s="22">
         <v>0.7</v>
       </c>
-      <c r="I14" s="73">
+      <c r="I14" s="59">
         <v>1944.7302</v>
       </c>
-      <c r="J14" s="73">
+      <c r="J14" s="59">
         <v>2434.9465</v>
       </c>
-      <c r="K14" s="73">
+      <c r="K14" s="59">
         <v>1889.8896999999999</v>
       </c>
-      <c r="L14" s="73">
+      <c r="L14" s="59">
         <v>2383.4546</v>
       </c>
-      <c r="M14" s="73">
+      <c r="M14" s="59">
         <v>1548.1909000000001</v>
       </c>
       <c r="N14" s="15"/>
@@ -36982,31 +36967,31 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="58" t="s">
+      <c r="A15" s="63" t="s">
         <v>274</v>
       </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
-      <c r="D15" s="58"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="58"/>
-      <c r="H15" s="68" t="s">
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="H15" s="72" t="s">
         <v>274</v>
       </c>
-      <c r="I15" s="68"/>
-      <c r="J15" s="68"/>
-      <c r="K15" s="68"/>
-      <c r="L15" s="68"/>
-      <c r="M15" s="68"/>
+      <c r="I15" s="72"/>
+      <c r="J15" s="72"/>
+      <c r="K15" s="72"/>
+      <c r="L15" s="72"/>
+      <c r="M15" s="72"/>
       <c r="N15" s="15"/>
-      <c r="O15" s="67" t="s">
+      <c r="O15" s="71" t="s">
         <v>274</v>
       </c>
-      <c r="P15" s="67"/>
-      <c r="Q15" s="67"/>
-      <c r="R15" s="67"/>
-      <c r="S15" s="67"/>
-      <c r="T15" s="67"/>
+      <c r="P15" s="71"/>
+      <c r="Q15" s="71"/>
+      <c r="R15" s="71"/>
+      <c r="S15" s="71"/>
+      <c r="T15" s="71"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" s="30" t="s">
@@ -37087,19 +37072,19 @@
       <c r="H17" s="22">
         <v>0.1</v>
       </c>
-      <c r="I17" s="73">
+      <c r="I17" s="59">
         <v>915.0363000000001</v>
       </c>
-      <c r="J17" s="73">
+      <c r="J17" s="59">
         <v>1252.3491000000001</v>
       </c>
-      <c r="K17" s="73">
+      <c r="K17" s="59">
         <v>1526.9779000000001</v>
       </c>
-      <c r="L17" s="73">
+      <c r="L17" s="59">
         <v>1618.3025</v>
       </c>
-      <c r="M17" s="74">
+      <c r="M17" s="60">
         <v>1835.0491</v>
       </c>
       <c r="N17" s="15"/>
@@ -37149,19 +37134,19 @@
       <c r="H18" s="22">
         <v>0.3</v>
       </c>
-      <c r="I18" s="73">
+      <c r="I18" s="59">
         <v>704.65199999999993</v>
       </c>
-      <c r="J18" s="73">
+      <c r="J18" s="59">
         <v>1151.441</v>
       </c>
-      <c r="K18" s="73">
+      <c r="K18" s="59">
         <v>1157.4152000000001</v>
       </c>
-      <c r="L18" s="73">
+      <c r="L18" s="59">
         <v>1071.6116</v>
       </c>
-      <c r="M18" s="73">
+      <c r="M18" s="59">
         <v>1108.5019</v>
       </c>
       <c r="N18" s="15"/>
@@ -37211,19 +37196,19 @@
       <c r="H19" s="22">
         <v>0.5</v>
       </c>
-      <c r="I19" s="73">
+      <c r="I19" s="59">
         <v>1138.7378999999999</v>
       </c>
-      <c r="J19" s="73">
+      <c r="J19" s="59">
         <v>1336.1958999999999</v>
       </c>
-      <c r="K19" s="73">
+      <c r="K19" s="59">
         <v>1775.0076999999999</v>
       </c>
-      <c r="L19" s="73">
+      <c r="L19" s="59">
         <v>1868.7972</v>
       </c>
-      <c r="M19" s="73">
+      <c r="M19" s="59">
         <v>1657.8720000000001</v>
       </c>
       <c r="N19" s="15"/>
@@ -37273,19 +37258,19 @@
       <c r="H20" s="22">
         <v>0.7</v>
       </c>
-      <c r="I20" s="73">
+      <c r="I20" s="59">
         <v>1268.0133000000001</v>
       </c>
-      <c r="J20" s="73">
+      <c r="J20" s="59">
         <v>1893.5635</v>
       </c>
-      <c r="K20" s="73">
+      <c r="K20" s="59">
         <v>1889.8896999999999</v>
       </c>
-      <c r="L20" s="73">
+      <c r="L20" s="59">
         <v>2383.4546</v>
       </c>
-      <c r="M20" s="73">
+      <c r="M20" s="59">
         <v>1548.1909000000001</v>
       </c>
       <c r="N20" s="15"/>
@@ -37314,40 +37299,40 @@
       <c r="AA20" s="43"/>
     </row>
     <row r="23" spans="1:109" x14ac:dyDescent="0.25">
-      <c r="A23" s="57"/>
-      <c r="B23" s="57"/>
-      <c r="C23" s="57"/>
-      <c r="D23" s="57"/>
-      <c r="E23" s="57"/>
-      <c r="F23" s="57"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
     </row>
     <row r="24" spans="1:109" x14ac:dyDescent="0.25">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="70" t="s">
         <v>357</v>
       </c>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="65"/>
-      <c r="E24" s="65"/>
-      <c r="F24" s="65"/>
-      <c r="H24" s="64" t="s">
+      <c r="B24" s="70"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="H24" s="69" t="s">
         <v>384</v>
       </c>
-      <c r="I24" s="64"/>
-      <c r="J24" s="64"/>
-      <c r="K24" s="64"/>
-      <c r="L24" s="64"/>
-      <c r="M24" s="64"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
     </row>
     <row r="25" spans="1:109" x14ac:dyDescent="0.25">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="B25" s="57"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="57"/>
-      <c r="E25" s="57"/>
-      <c r="F25" s="57"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
     </row>
     <row r="26" spans="1:109" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
@@ -37368,7 +37353,7 @@
       <c r="F26" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H26" s="63" t="s">
+      <c r="H26" s="68" t="s">
         <v>278</v>
       </c>
       <c r="I26" t="s">
@@ -37400,7 +37385,7 @@
       <c r="F27">
         <v>32229</v>
       </c>
-      <c r="H27" s="63"/>
+      <c r="H27" s="68"/>
       <c r="I27" t="s">
         <v>5</v>
       </c>
@@ -37724,7 +37709,7 @@
       <c r="F28">
         <v>32938</v>
       </c>
-      <c r="H28" s="63"/>
+      <c r="H28" s="68"/>
       <c r="I28" t="s">
         <v>6</v>
       </c>
@@ -38072,15 +38057,15 @@
       <c r="H30" s="23"/>
     </row>
     <row r="31" spans="1:109" x14ac:dyDescent="0.25">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="H31" s="63" t="s">
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="H31" s="68" t="s">
         <v>280</v>
       </c>
       <c r="I31" t="s">
@@ -38112,7 +38097,7 @@
       <c r="F32" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H32" s="63"/>
+      <c r="H32" s="68"/>
       <c r="I32" t="s">
         <v>5</v>
       </c>
@@ -38436,7 +38421,7 @@
       <c r="F33">
         <v>32511</v>
       </c>
-      <c r="H33" s="63"/>
+      <c r="H33" s="68"/>
       <c r="I33" t="s">
         <v>6</v>
       </c>
@@ -38802,7 +38787,7 @@
       <c r="F36">
         <v>28377</v>
       </c>
-      <c r="H36" s="63" t="s">
+      <c r="H36" s="68" t="s">
         <v>281</v>
       </c>
       <c r="I36" t="s">
@@ -38816,15 +38801,15 @@
       </c>
     </row>
     <row r="37" spans="1:109" x14ac:dyDescent="0.25">
-      <c r="A37" s="57" t="s">
+      <c r="A37" s="61" t="s">
         <v>274</v>
       </c>
-      <c r="B37" s="57"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="57"/>
-      <c r="E37" s="57"/>
-      <c r="F37" s="57"/>
-      <c r="H37" s="63"/>
+      <c r="B37" s="61"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="61"/>
+      <c r="E37" s="61"/>
+      <c r="F37" s="61"/>
+      <c r="H37" s="68"/>
       <c r="I37" t="s">
         <v>5</v>
       </c>
@@ -39148,7 +39133,7 @@
       <c r="F38" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="H38" s="63"/>
+      <c r="H38" s="68"/>
       <c r="I38" t="s">
         <v>6</v>
       </c>
@@ -39493,7 +39478,7 @@
       <c r="F40">
         <v>33349</v>
       </c>
-      <c r="H40" s="63" t="s">
+      <c r="H40" s="68" t="s">
         <v>282</v>
       </c>
       <c r="I40" t="s">
@@ -39525,7 +39510,7 @@
       <c r="F41">
         <v>27821</v>
       </c>
-      <c r="H41" s="63"/>
+      <c r="H41" s="68"/>
       <c r="I41" t="s">
         <v>5</v>
       </c>
@@ -39849,7 +39834,7 @@
       <c r="F42">
         <v>28659</v>
       </c>
-      <c r="H42" s="63"/>
+      <c r="H42" s="68"/>
       <c r="I42" t="s">
         <v>6</v>
       </c>
@@ -40156,6 +40141,18 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="H2:M2"/>
+    <mergeCell ref="O2:T2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="H3:M3"/>
+    <mergeCell ref="O3:T3"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="H9:M9"/>
+    <mergeCell ref="O9:T9"/>
+    <mergeCell ref="A15:F15"/>
+    <mergeCell ref="H15:M15"/>
+    <mergeCell ref="O15:T15"/>
     <mergeCell ref="H36:H38"/>
     <mergeCell ref="A37:F37"/>
     <mergeCell ref="H40:H42"/>
@@ -40166,18 +40163,6 @@
     <mergeCell ref="H26:H28"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="H31:H33"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="H9:M9"/>
-    <mergeCell ref="O9:T9"/>
-    <mergeCell ref="A15:F15"/>
-    <mergeCell ref="H15:M15"/>
-    <mergeCell ref="O15:T15"/>
-    <mergeCell ref="A2:F2"/>
-    <mergeCell ref="H2:M2"/>
-    <mergeCell ref="O2:T2"/>
-    <mergeCell ref="A3:F3"/>
-    <mergeCell ref="H3:M3"/>
-    <mergeCell ref="O3:T3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -40201,89 +40186,89 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="G1" s="57" t="s">
+      <c r="G1" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="69" t="s">
+      <c r="A2" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="69"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="H2" s="70" t="s">
+      <c r="B2" s="73"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="H2" s="74" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="O2" s="64" t="s">
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+      <c r="M2" s="74"/>
+      <c r="O2" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="64"/>
-      <c r="T2" s="64"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+      <c r="R2" s="69"/>
+      <c r="S2" s="69"/>
+      <c r="T2" s="69"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="70" t="s">
         <v>277</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="H3" s="65" t="s">
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="H3" s="70" t="s">
         <v>277</v>
       </c>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="O3" s="65" t="s">
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="O3" s="70" t="s">
         <v>357</v>
       </c>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="70"/>
+      <c r="T3" s="70"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="57"/>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="H4" s="57" t="s">
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="H4" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="O4" s="57" t="s">
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="O4" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57"/>
-      <c r="T4" s="57"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="61"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="54" t="s">
@@ -40571,31 +40556,31 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="67" t="s">
+      <c r="A10" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="67"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="H10" s="67" t="s">
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="H10" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="I10" s="67"/>
-      <c r="J10" s="67"/>
-      <c r="K10" s="67"/>
-      <c r="L10" s="67"/>
-      <c r="M10" s="67"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
+      <c r="K10" s="71"/>
+      <c r="L10" s="71"/>
+      <c r="M10" s="71"/>
       <c r="N10" s="15"/>
-      <c r="O10" s="67" t="s">
+      <c r="O10" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="P10" s="67"/>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67"/>
-      <c r="S10" s="67"/>
-      <c r="T10" s="67"/>
+      <c r="P10" s="71"/>
+      <c r="Q10" s="71"/>
+      <c r="R10" s="71"/>
+      <c r="S10" s="71"/>
+      <c r="T10" s="71"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
@@ -40883,31 +40868,31 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="67" t="s">
+      <c r="A16" s="71" t="s">
         <v>274</v>
       </c>
-      <c r="B16" s="67"/>
-      <c r="C16" s="67"/>
-      <c r="D16" s="67"/>
-      <c r="E16" s="67"/>
-      <c r="F16" s="67"/>
-      <c r="H16" s="67" t="s">
+      <c r="B16" s="71"/>
+      <c r="C16" s="71"/>
+      <c r="D16" s="71"/>
+      <c r="E16" s="71"/>
+      <c r="F16" s="71"/>
+      <c r="H16" s="71" t="s">
         <v>274</v>
       </c>
-      <c r="I16" s="67"/>
-      <c r="J16" s="67"/>
-      <c r="K16" s="67"/>
-      <c r="L16" s="67"/>
-      <c r="M16" s="67"/>
+      <c r="I16" s="71"/>
+      <c r="J16" s="71"/>
+      <c r="K16" s="71"/>
+      <c r="L16" s="71"/>
+      <c r="M16" s="71"/>
       <c r="N16" s="15"/>
-      <c r="O16" s="67" t="s">
+      <c r="O16" s="71" t="s">
         <v>274</v>
       </c>
-      <c r="P16" s="67"/>
-      <c r="Q16" s="67"/>
-      <c r="R16" s="67"/>
-      <c r="S16" s="67"/>
-      <c r="T16" s="67"/>
+      <c r="P16" s="71"/>
+      <c r="Q16" s="71"/>
+      <c r="R16" s="71"/>
+      <c r="S16" s="71"/>
+      <c r="T16" s="71"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="53" t="s">
@@ -41196,6 +41181,11 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="O2:T2"/>
+    <mergeCell ref="O3:T3"/>
+    <mergeCell ref="O4:T4"/>
+    <mergeCell ref="O10:T10"/>
+    <mergeCell ref="O16:T16"/>
     <mergeCell ref="A16:F16"/>
     <mergeCell ref="H4:M4"/>
     <mergeCell ref="H10:M10"/>
@@ -41207,11 +41197,6 @@
     <mergeCell ref="H3:M3"/>
     <mergeCell ref="A4:F4"/>
     <mergeCell ref="A10:F10"/>
-    <mergeCell ref="O2:T2"/>
-    <mergeCell ref="O3:T3"/>
-    <mergeCell ref="O4:T4"/>
-    <mergeCell ref="O10:T10"/>
-    <mergeCell ref="O16:T16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>